<commit_message>
Update plan de test et execution_programme
</commit_message>
<xml_diff>
--- a/Documents_Qualite_Developpement/Plan de test 2048.xlsx
+++ b/Documents_Qualite_Developpement/Plan de test 2048.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t xml:space="preserve">Nom du projet </t>
   </si>
@@ -70,10 +70,10 @@
     <t xml:space="preserve">Nombre d'essai</t>
   </si>
   <si>
-    <t xml:space="preserve">Boutons radios de paramètres dans la page menu vide par défaut.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les boutons radio doivent être vides au chargement de la page menu.</t>
+    <t xml:space="preserve">Boutons radios 2048 et 4x4 cochés par défaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les boutons radio doivent être cochés au chargement de la page menu.</t>
   </si>
   <si>
     <t xml:space="preserve">Boutons radios de paramètres dans la page menu.</t>
@@ -100,10 +100,10 @@
     <t xml:space="preserve">Utilisation toujours agréable de la page menu peu importe la résolution de l’écran.</t>
   </si>
   <si>
-    <t xml:space="preserve">Grille de jeu vide par défaut.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afficher correctement une grille de jeu vide au chargement de la page de jeu.</t>
+    <t xml:space="preserve">Grille de jeu avec deux blocs par défaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afficher correctement une grille de jeu avec deux blocs au chargement de la page de jeu.</t>
   </si>
   <si>
     <t xml:space="preserve">Déplacement des blocs de 2048 avec les flèches directionnelles.</t>
@@ -130,6 +130,12 @@
     <t xml:space="preserve">Animation qui rend les déplacements des blocs plus fluide.</t>
   </si>
   <si>
+    <t xml:space="preserve">Pas d’animations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développer les animations</t>
+  </si>
+  <si>
     <t xml:space="preserve">Affichage du score en temps réel.</t>
   </si>
   <si>
@@ -154,12 +160,21 @@
     <t xml:space="preserve">Arrêter la partie et afficher que la partie est gagné.</t>
   </si>
   <si>
+    <t xml:space="preserve">Victoire pas détectée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrêter la partie quand il y a un 2048 sur la grille pour le mode classique</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stockage du (high) score (seulement en mode 4x4)</t>
   </si>
   <si>
     <t xml:space="preserve">Envoyer le pseudonyme et le score du joueur s’il est à stocker dans le fichier des high score (uniquement en mode 4x4).</t>
   </si>
   <si>
+    <t xml:space="preserve">fichier csv non trouvé</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bouton de consultation des high scores depuis la page de jeu.</t>
   </si>
   <si>
@@ -172,12 +187,24 @@
     <t xml:space="preserve">Relance une nouvelle partie.</t>
   </si>
   <si>
+    <t xml:space="preserve">Bouton non présent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter le bouton</t>
+  </si>
+  <si>
     <t xml:space="preserve">Responsive de la page jeu.</t>
   </si>
   <si>
     <t xml:space="preserve">Utilisation toujours agréable de la page jeu peu importe la résolution de l’écran.</t>
   </si>
   <si>
+    <t xml:space="preserve">Responsive pas adapté à toutes les tailles d’écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapetisser la grille et les blocs en fonction de l’écran</t>
+  </si>
+  <si>
     <t xml:space="preserve">Affichage par défaut du mode infini dans la page high score.</t>
   </si>
   <si>
@@ -233,16 +260,18 @@
   </si>
   <si>
     <t xml:space="preserve">Utilisation toujours agréable de la page high score peu importe la résolution de l’écran.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapetisser le tableau en fonction de l’écran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -489,7 +518,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,7 +538,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -558,7 +587,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -584,7 +613,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE699"/>
+          <fgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9966"/>
         </patternFill>
       </fill>
     </dxf>
@@ -676,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -820,15 +856,15 @@
       <c r="C10" s="10"/>
       <c r="D10" s="13" t="n">
         <f aca="false">SUM(D16:D116)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E10" s="13" t="n">
         <f aca="false">SUM(E16:E116)</f>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F10" s="13" t="n">
         <f aca="false">SUM(F16:F116)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -848,15 +884,15 @@
       <c r="C11" s="10"/>
       <c r="D11" s="14" t="str">
         <f aca="false">CONCATENATE("Soit ",TEXT( D10*100/A10,"0"),"%")</f>
-        <v>Soit 0%</v>
+        <v>Soit 64%</v>
       </c>
       <c r="E11" s="14" t="str">
         <f aca="false">CONCATENATE("Soit ",TEXT( E10*100/A10,"0"),"%")</f>
-        <v>Soit 100%</v>
+        <v>Soit 0%</v>
       </c>
       <c r="F11" s="14" t="str">
         <f aca="false">CONCATENATE("Soit ",TEXT( F10*100/A10,"0"),"%")</f>
-        <v>Soit 0%</v>
+        <v>Soit 36%</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -947,16 +983,18 @@
       <c r="C16" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D16" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21"/>
       <c r="F16" s="22"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
         <v>18</v>
       </c>
@@ -966,14 +1004,16 @@
       <c r="C17" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D17" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="21"/>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
+      <c r="I17" s="24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
@@ -985,14 +1025,16 @@
       <c r="C18" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D18" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
+      <c r="I18" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
@@ -1004,14 +1046,16 @@
       <c r="C19" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D19" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="21"/>
       <c r="F19" s="22"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
@@ -1023,14 +1067,16 @@
       <c r="C20" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D20" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="21"/>
       <c r="F20" s="22"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
+      <c r="I20" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
@@ -1053,14 +1099,16 @@
       <c r="C22" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D22" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="21"/>
       <c r="F22" s="22"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
+      <c r="I22" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
@@ -1072,14 +1120,16 @@
       <c r="C23" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D23" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
+      <c r="I23" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
@@ -1091,16 +1141,16 @@
       <c r="C24" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D24" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
         <v>32</v>
       </c>
@@ -1110,14 +1160,16 @@
       <c r="C25" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D25" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
+      <c r="I25" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
@@ -1130,165 +1182,201 @@
         <v>45616</v>
       </c>
       <c r="D26" s="20"/>
-      <c r="E26" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C27" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D27" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="21"/>
       <c r="F27" s="22"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
+      <c r="I27" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D28" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="21"/>
       <c r="F28" s="22"/>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
+      <c r="I28" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C29" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D29" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="21"/>
       <c r="F29" s="22"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
-      <c r="I29" s="24"/>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C30" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D30" s="20"/>
-      <c r="E30" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" s="24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C31" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D31" s="20"/>
-      <c r="E31" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
+      <c r="I31" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C32" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D32" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="21"/>
       <c r="F32" s="22"/>
       <c r="G32" s="23"/>
       <c r="H32" s="23"/>
-      <c r="I32" s="24"/>
+      <c r="I32" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C33" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D33" s="20"/>
-      <c r="E33" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C34" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D34" s="20"/>
-      <c r="E34" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="23"/>
@@ -1301,195 +1389,235 @@
       <c r="H35" s="23"/>
       <c r="I35" s="24"/>
     </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C36" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D36" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="21"/>
       <c r="F36" s="22"/>
       <c r="G36" s="23"/>
       <c r="H36" s="23"/>
-      <c r="I36" s="24"/>
+      <c r="I36" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C37" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D37" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="21"/>
       <c r="F37" s="22"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23"/>
-      <c r="I37" s="24"/>
+      <c r="I37" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C38" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D38" s="20"/>
-      <c r="E38" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="24"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C39" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D39" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="21"/>
       <c r="F39" s="22"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
-      <c r="I39" s="24"/>
+      <c r="I39" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C40" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D40" s="20"/>
-      <c r="E40" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="24"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I40" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="23" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C41" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D41" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="21"/>
       <c r="F41" s="22"/>
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="23" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C42" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D42" s="20"/>
-      <c r="E42" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="24"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C43" s="19" t="n">
         <v>45616</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="D43" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="21"/>
       <c r="F43" s="22"/>
       <c r="G43" s="23"/>
       <c r="H43" s="23"/>
-      <c r="I43" s="24"/>
+      <c r="I43" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="23" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C44" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D44" s="20"/>
-      <c r="E44" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="24"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="23" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C45" s="19" t="n">
         <v>45616</v>
       </c>
       <c r="D45" s="20"/>
-      <c r="E45" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="24"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I45" s="24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="23"/>

</xml_diff>